<commit_message>
adding data and parsing it
</commit_message>
<xml_diff>
--- a/Data/2016/03_March/20160317_NCBI_Mass_spec_pb1710_search/20160316_Bethany_QE_0060_Andrew_Native_TMT_2_YeastDatabase_native.xlsx
+++ b/Data/2016/03_March/20160317_NCBI_Mass_spec_pb1710_search/20160316_Bethany_QE_0060_Andrew_Native_TMT_2_YeastDatabase_native.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-37000" yWindow="80" windowWidth="35520" windowHeight="20160" activeTab="1"/>
+    <workbookView xWindow="2400" yWindow="560" windowWidth="19380" windowHeight="12960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -876,11 +876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2103499048"/>
-        <c:axId val="-2127181112"/>
+        <c:axId val="2122988664"/>
+        <c:axId val="2129640392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2103499048"/>
+        <c:axId val="2122988664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,12 +890,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127181112"/>
+        <c:crossAx val="2129640392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127181112"/>
+        <c:axId val="2129640392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,7 +905,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103499048"/>
+        <c:crossAx val="2122988664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5576,8 +5576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.1640625" defaultRowHeight="12" outlineLevelRow="1" x14ac:dyDescent="0"/>
@@ -7342,7 +7342,7 @@
         <v>1.2501264984207021</v>
       </c>
       <c r="F39">
-        <f t="shared" ref="E39:L39" si="0">1/F27</f>
+        <f t="shared" ref="F39:L39" si="0">1/F27</f>
         <v>1.3575188964551392</v>
       </c>
       <c r="G39">
@@ -7642,39 +7642,39 @@
         <v>1</v>
       </c>
       <c r="C50">
-        <f>D39*D49</f>
+        <f t="shared" ref="C50:K50" si="3">D39*D49</f>
         <v>0.63593420524979982</v>
       </c>
       <c r="D50">
-        <f>E39*E49</f>
+        <f t="shared" si="3"/>
         <v>0.98547052461292561</v>
       </c>
       <c r="E50">
-        <f>F39*F49</f>
+        <f t="shared" si="3"/>
         <v>1.0559078611874448</v>
       </c>
       <c r="F50">
-        <f>G39*G49</f>
+        <f t="shared" si="3"/>
         <v>1.2531832766631399</v>
       </c>
       <c r="G50">
-        <f>H39*H49</f>
+        <f t="shared" si="3"/>
         <v>0.99985147031306287</v>
       </c>
       <c r="H50">
-        <f>I39*I49</f>
+        <f t="shared" si="3"/>
         <v>0.74202019608371583</v>
       </c>
       <c r="I50">
-        <f>J39*J49</f>
+        <f t="shared" si="3"/>
         <v>1.0306718697901094</v>
       </c>
       <c r="J50">
-        <f>K39*K49</f>
+        <f t="shared" si="3"/>
         <v>0.89097460494555702</v>
       </c>
       <c r="K50">
-        <f>L39*L49</f>
+        <f t="shared" si="3"/>
         <v>0.83695633652891754</v>
       </c>
     </row>
@@ -7731,31 +7731,31 @@
         <v>1.0018407575572983</v>
       </c>
       <c r="E52">
-        <f t="shared" ref="D52:K52" si="3">F39*E51</f>
+        <f t="shared" ref="E52:K52" si="4">F39*E51</f>
         <v>1.0482726986749586</v>
       </c>
       <c r="F52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2679746821229891</v>
       </c>
       <c r="G52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0303612657239964</v>
       </c>
       <c r="H52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.74354007134495581</v>
       </c>
       <c r="I52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0510502409388118</v>
       </c>
       <c r="J52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.85823278310230677</v>
       </c>
       <c r="K52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.81687235038492412</v>
       </c>
     </row>

</xml_diff>